<commit_message>
analyze the data for well 1,2,3
</commit_message>
<xml_diff>
--- a/datasets/well1.xlsx
+++ b/datasets/well1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my documents\dars\siri\Production\05. Esfand Field (SIE)\WPE1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliyu\Documents\Machine Learning\Work\back-allocation-using-machine-learning\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B8F35CE-9138-4602-99D9-694897C0C380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB2CB6A-2577-4EBF-A98B-108205A27D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="17535" windowHeight="9090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full History" sheetId="4" r:id="rId1"/>
@@ -3289,7 +3289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -3513,11 +3513,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3766,50 +3777,39 @@
     <xf numFmtId="1" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="20" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3841,38 +3841,50 @@
     <xf numFmtId="0" fontId="11" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="20" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3880,7 +3892,12 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="8" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -44473,9 +44490,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -44513,9 +44530,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -44548,9 +44565,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -44583,9 +44617,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -44762,8 +44813,8 @@
   <dimension ref="A1:AC210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:M1"/>
+      <pane ySplit="3" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -44789,38 +44840,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A1" s="110"/>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="112"/>
+      <c r="A1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="92"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="113" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="114"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="94"/>
     </row>
     <row r="3" spans="1:13" s="18" customFormat="1" ht="36" customHeight="1">
       <c r="A3" s="24" t="s">
@@ -44867,8 +44918,8 @@
       <c r="A4" s="36">
         <v>36178</v>
       </c>
-      <c r="B4" s="36">
-        <v>36178</v>
+      <c r="B4" s="123">
+        <v>36179</v>
       </c>
       <c r="C4" s="37">
         <v>44</v>
@@ -44906,8 +44957,8 @@
       <c r="A5" s="46">
         <v>36196</v>
       </c>
-      <c r="B5" s="46">
-        <v>36196</v>
+      <c r="B5" s="124">
+        <v>36180</v>
       </c>
       <c r="C5" s="47">
         <v>50</v>
@@ -44946,8 +44997,8 @@
       <c r="A6" s="46">
         <v>36197</v>
       </c>
-      <c r="B6" s="46">
-        <v>36197</v>
+      <c r="B6" s="124">
+        <v>36181</v>
       </c>
       <c r="C6" s="47">
         <v>55</v>
@@ -44986,8 +45037,8 @@
       <c r="A7" s="46">
         <v>36199</v>
       </c>
-      <c r="B7" s="46">
-        <v>36199</v>
+      <c r="B7" s="124">
+        <v>36182</v>
       </c>
       <c r="C7" s="47">
         <v>55</v>
@@ -45026,8 +45077,8 @@
       <c r="A8" s="46">
         <v>36200</v>
       </c>
-      <c r="B8" s="46">
-        <v>36200</v>
+      <c r="B8" s="124">
+        <v>36185</v>
       </c>
       <c r="C8" s="47">
         <v>55</v>
@@ -45066,8 +45117,8 @@
       <c r="A9" s="46">
         <v>36202</v>
       </c>
-      <c r="B9" s="46">
-        <v>36202</v>
+      <c r="B9" s="124">
+        <v>36186</v>
       </c>
       <c r="C9" s="47">
         <v>55</v>
@@ -45106,8 +45157,8 @@
       <c r="A10" s="46">
         <v>36207</v>
       </c>
-      <c r="B10" s="46">
-        <v>36207</v>
+      <c r="B10" s="124">
+        <v>36187</v>
       </c>
       <c r="C10" s="47">
         <v>55</v>
@@ -45146,8 +45197,8 @@
       <c r="A11" s="46">
         <v>36208</v>
       </c>
-      <c r="B11" s="46">
-        <v>36208</v>
+      <c r="B11" s="124">
+        <v>36188</v>
       </c>
       <c r="C11" s="47">
         <v>55</v>
@@ -45186,8 +45237,8 @@
       <c r="A12" s="46">
         <v>36209</v>
       </c>
-      <c r="B12" s="46">
-        <v>36209</v>
+      <c r="B12" s="124">
+        <v>36191</v>
       </c>
       <c r="C12" s="47">
         <v>50</v>
@@ -45226,8 +45277,8 @@
       <c r="A13" s="46">
         <v>36214</v>
       </c>
-      <c r="B13" s="46">
-        <v>36214</v>
+      <c r="B13" s="124">
+        <v>36193</v>
       </c>
       <c r="C13" s="47">
         <v>45</v>
@@ -45266,8 +45317,8 @@
       <c r="A14" s="46">
         <v>36216</v>
       </c>
-      <c r="B14" s="46">
-        <v>36216</v>
+      <c r="B14" s="124">
+        <v>36194</v>
       </c>
       <c r="C14" s="47">
         <v>45</v>
@@ -45306,8 +45357,8 @@
       <c r="A15" s="46">
         <v>36217</v>
       </c>
-      <c r="B15" s="46">
-        <v>36217</v>
+      <c r="B15" s="124">
+        <v>36197</v>
       </c>
       <c r="C15" s="47">
         <v>45</v>
@@ -45346,8 +45397,8 @@
       <c r="A16" s="46">
         <v>36227</v>
       </c>
-      <c r="B16" s="46">
-        <v>36227</v>
+      <c r="B16" s="124">
+        <v>36199</v>
       </c>
       <c r="C16" s="47">
         <v>30</v>
@@ -45388,8 +45439,8 @@
       <c r="A17" s="46">
         <v>36242</v>
       </c>
-      <c r="B17" s="46">
-        <v>36242</v>
+      <c r="B17" s="124">
+        <v>36201</v>
       </c>
       <c r="C17" s="47">
         <v>55</v>
@@ -45428,8 +45479,8 @@
       <c r="A18" s="46">
         <v>36243</v>
       </c>
-      <c r="B18" s="46">
-        <v>36243</v>
+      <c r="B18" s="124">
+        <v>36207</v>
       </c>
       <c r="C18" s="47">
         <v>55</v>
@@ -45470,8 +45521,8 @@
       <c r="A19" s="46">
         <v>36245</v>
       </c>
-      <c r="B19" s="46">
-        <v>36245</v>
+      <c r="B19" s="124">
+        <v>36208</v>
       </c>
       <c r="C19" s="47">
         <v>45</v>
@@ -45512,8 +45563,8 @@
       <c r="A20" s="46">
         <v>36248</v>
       </c>
-      <c r="B20" s="46">
-        <v>36248</v>
+      <c r="B20" s="124">
+        <v>36209</v>
       </c>
       <c r="C20" s="47">
         <v>40</v>
@@ -45554,8 +45605,8 @@
       <c r="A21" s="46">
         <v>36251</v>
       </c>
-      <c r="B21" s="46">
-        <v>36251</v>
+      <c r="B21" s="124">
+        <v>36211</v>
       </c>
       <c r="C21" s="47">
         <v>36</v>
@@ -45596,8 +45647,8 @@
       <c r="A22" s="46">
         <v>36256</v>
       </c>
-      <c r="B22" s="46">
-        <v>36256</v>
+      <c r="B22" s="124">
+        <v>36213</v>
       </c>
       <c r="C22" s="47">
         <v>36</v>
@@ -45638,8 +45689,8 @@
       <c r="A23" s="46">
         <v>36261</v>
       </c>
-      <c r="B23" s="46">
-        <v>36261</v>
+      <c r="B23" s="124">
+        <v>36217</v>
       </c>
       <c r="C23" s="47">
         <v>36</v>
@@ -45680,8 +45731,8 @@
       <c r="A24" s="46">
         <v>36267</v>
       </c>
-      <c r="B24" s="46">
-        <v>36267</v>
+      <c r="B24" s="124">
+        <v>36218</v>
       </c>
       <c r="C24" s="47">
         <v>36</v>
@@ -45722,8 +45773,8 @@
       <c r="A25" s="46">
         <v>36272</v>
       </c>
-      <c r="B25" s="46">
-        <v>36272</v>
+      <c r="B25" s="124">
+        <v>36222</v>
       </c>
       <c r="C25" s="47">
         <v>36</v>
@@ -45764,8 +45815,8 @@
       <c r="A26" s="46">
         <v>36275</v>
       </c>
-      <c r="B26" s="46">
-        <v>36275</v>
+      <c r="B26" s="124">
+        <v>36226</v>
       </c>
       <c r="C26" s="47">
         <v>36</v>
@@ -45806,8 +45857,8 @@
       <c r="A27" s="46">
         <v>36281</v>
       </c>
-      <c r="B27" s="46">
-        <v>36281</v>
+      <c r="B27" s="124">
+        <v>36227</v>
       </c>
       <c r="C27" s="47">
         <v>36</v>
@@ -45848,8 +45899,8 @@
       <c r="A28" s="46">
         <v>36284</v>
       </c>
-      <c r="B28" s="46">
-        <v>36284</v>
+      <c r="B28" s="124">
+        <v>36228</v>
       </c>
       <c r="C28" s="47">
         <v>36</v>
@@ -45890,8 +45941,8 @@
       <c r="A29" s="46">
         <v>36288</v>
       </c>
-      <c r="B29" s="46">
-        <v>36288</v>
+      <c r="B29" s="124">
+        <v>36233</v>
       </c>
       <c r="C29" s="47">
         <v>36</v>
@@ -45932,8 +45983,8 @@
       <c r="A30" s="46">
         <v>36291</v>
       </c>
-      <c r="B30" s="46">
-        <v>36291</v>
+      <c r="B30" s="124">
+        <v>36234</v>
       </c>
       <c r="C30" s="47">
         <v>36</v>
@@ -45972,8 +46023,8 @@
       <c r="A31" s="46">
         <v>36294</v>
       </c>
-      <c r="B31" s="46">
-        <v>36294</v>
+      <c r="B31" s="124">
+        <v>36235</v>
       </c>
       <c r="C31" s="47">
         <v>36</v>
@@ -46014,8 +46065,8 @@
       <c r="A32" s="46">
         <v>36298</v>
       </c>
-      <c r="B32" s="46">
-        <v>36298</v>
+      <c r="B32" s="124">
+        <v>36236</v>
       </c>
       <c r="C32" s="47">
         <v>48</v>
@@ -46056,8 +46107,8 @@
       <c r="A33" s="46">
         <v>36299</v>
       </c>
-      <c r="B33" s="46">
-        <v>36299</v>
+      <c r="B33" s="124">
+        <v>36244</v>
       </c>
       <c r="C33" s="47">
         <v>48</v>
@@ -46096,8 +46147,8 @@
       <c r="A34" s="46">
         <v>36300</v>
       </c>
-      <c r="B34" s="46">
-        <v>36300</v>
+      <c r="B34" s="124">
+        <v>36249</v>
       </c>
       <c r="C34" s="47">
         <v>48</v>
@@ -46138,8 +46189,8 @@
       <c r="A35" s="46">
         <v>36304</v>
       </c>
-      <c r="B35" s="46">
-        <v>36304</v>
+      <c r="B35" s="124">
+        <v>36251</v>
       </c>
       <c r="C35" s="47">
         <v>48</v>
@@ -46180,8 +46231,8 @@
       <c r="A36" s="46">
         <v>36307</v>
       </c>
-      <c r="B36" s="46">
-        <v>36307</v>
+      <c r="B36" s="124">
+        <v>36257</v>
       </c>
       <c r="C36" s="47">
         <v>48</v>
@@ -46222,8 +46273,8 @@
       <c r="A37" s="46">
         <v>36311</v>
       </c>
-      <c r="B37" s="46">
-        <v>36311</v>
+      <c r="B37" s="124">
+        <v>36262</v>
       </c>
       <c r="C37" s="47">
         <v>48</v>
@@ -46264,8 +46315,8 @@
       <c r="A38" s="46">
         <v>36316</v>
       </c>
-      <c r="B38" s="46">
-        <v>36316</v>
+      <c r="B38" s="124">
+        <v>36265</v>
       </c>
       <c r="C38" s="47">
         <v>48</v>
@@ -46306,8 +46357,8 @@
       <c r="A39" s="46">
         <v>36321</v>
       </c>
-      <c r="B39" s="46">
-        <v>36321</v>
+      <c r="B39" s="124">
+        <v>36268</v>
       </c>
       <c r="C39" s="47">
         <v>48</v>
@@ -46348,8 +46399,8 @@
       <c r="A40" s="46">
         <v>36325</v>
       </c>
-      <c r="B40" s="46">
-        <v>36325</v>
+      <c r="B40" s="124">
+        <v>36269</v>
       </c>
       <c r="C40" s="47">
         <v>48</v>
@@ -46390,8 +46441,8 @@
       <c r="A41" s="46">
         <v>36330</v>
       </c>
-      <c r="B41" s="46">
-        <v>36330</v>
+      <c r="B41" s="124">
+        <v>36272</v>
       </c>
       <c r="C41" s="47">
         <v>44</v>
@@ -46432,8 +46483,8 @@
       <c r="A42" s="46">
         <v>36331</v>
       </c>
-      <c r="B42" s="46">
-        <v>36331</v>
+      <c r="B42" s="124">
+        <v>36276</v>
       </c>
       <c r="C42" s="47">
         <v>44</v>
@@ -46472,8 +46523,8 @@
       <c r="A43" s="46">
         <v>36335</v>
       </c>
-      <c r="B43" s="46">
-        <v>36335</v>
+      <c r="B43" s="124">
+        <v>36280</v>
       </c>
       <c r="C43" s="47">
         <v>44</v>
@@ -46514,8 +46565,8 @@
       <c r="A44" s="46">
         <v>36338</v>
       </c>
-      <c r="B44" s="46">
-        <v>36338</v>
+      <c r="B44" s="124">
+        <v>36285</v>
       </c>
       <c r="C44" s="47">
         <v>44</v>
@@ -46556,8 +46607,8 @@
       <c r="A45" s="46">
         <v>36342</v>
       </c>
-      <c r="B45" s="46">
-        <v>36342</v>
+      <c r="B45" s="124">
+        <v>36288</v>
       </c>
       <c r="C45" s="47">
         <v>44</v>
@@ -46598,8 +46649,8 @@
       <c r="A46" s="46">
         <v>36346</v>
       </c>
-      <c r="B46" s="46">
-        <v>36346</v>
+      <c r="B46" s="124">
+        <v>36291</v>
       </c>
       <c r="C46" s="47">
         <v>44</v>
@@ -46640,8 +46691,8 @@
       <c r="A47" s="46">
         <v>36354</v>
       </c>
-      <c r="B47" s="46">
-        <v>36354</v>
+      <c r="B47" s="124">
+        <v>36295</v>
       </c>
       <c r="C47" s="47">
         <v>44</v>
@@ -46682,8 +46733,8 @@
       <c r="A48" s="46">
         <v>36361</v>
       </c>
-      <c r="B48" s="46">
-        <v>36361</v>
+      <c r="B48" s="124">
+        <v>36298</v>
       </c>
       <c r="C48" s="47">
         <v>44</v>
@@ -46724,8 +46775,8 @@
       <c r="A49" s="46">
         <v>36365</v>
       </c>
-      <c r="B49" s="46">
-        <v>36365</v>
+      <c r="B49" s="124">
+        <v>36303</v>
       </c>
       <c r="C49" s="47">
         <v>44</v>
@@ -46766,8 +46817,8 @@
       <c r="A50" s="46">
         <v>36369</v>
       </c>
-      <c r="B50" s="46">
-        <v>36369</v>
+      <c r="B50" s="124">
+        <v>36306</v>
       </c>
       <c r="C50" s="47">
         <v>44</v>
@@ -46806,8 +46857,8 @@
       <c r="A51" s="46">
         <v>36375</v>
       </c>
-      <c r="B51" s="46">
-        <v>36375</v>
+      <c r="B51" s="124">
+        <v>36310</v>
       </c>
       <c r="C51" s="56">
         <v>44</v>
@@ -46848,8 +46899,8 @@
       <c r="A52" s="46">
         <v>36377</v>
       </c>
-      <c r="B52" s="46">
-        <v>36377</v>
+      <c r="B52" s="124">
+        <v>36315</v>
       </c>
       <c r="C52" s="56">
         <v>44</v>
@@ -46890,8 +46941,8 @@
       <c r="A53" s="46">
         <v>36382</v>
       </c>
-      <c r="B53" s="46">
-        <v>36382</v>
+      <c r="B53" s="124">
+        <v>36320</v>
       </c>
       <c r="C53" s="56">
         <v>44</v>
@@ -46932,8 +46983,8 @@
       <c r="A54" s="46">
         <v>36386</v>
       </c>
-      <c r="B54" s="46">
-        <v>36386</v>
+      <c r="B54" s="124">
+        <v>36324</v>
       </c>
       <c r="C54" s="56">
         <v>44</v>
@@ -46974,8 +47025,8 @@
       <c r="A55" s="46">
         <v>36403</v>
       </c>
-      <c r="B55" s="46">
-        <v>36403</v>
+      <c r="B55" s="124">
+        <v>36327</v>
       </c>
       <c r="C55" s="56">
         <v>44</v>
@@ -47016,8 +47067,8 @@
       <c r="A56" s="46">
         <v>36412</v>
       </c>
-      <c r="B56" s="46">
-        <v>36412</v>
+      <c r="B56" s="124">
+        <v>36331</v>
       </c>
       <c r="C56" s="56">
         <v>44</v>
@@ -47058,8 +47109,8 @@
       <c r="A57" s="46">
         <v>36416</v>
       </c>
-      <c r="B57" s="46">
-        <v>36416</v>
+      <c r="B57" s="124">
+        <v>36335</v>
       </c>
       <c r="C57" s="56">
         <v>44</v>
@@ -47100,8 +47151,8 @@
       <c r="A58" s="46">
         <v>36419</v>
       </c>
-      <c r="B58" s="46">
-        <v>36419</v>
+      <c r="B58" s="124">
+        <v>36339</v>
       </c>
       <c r="C58" s="56">
         <v>44</v>
@@ -47142,8 +47193,8 @@
       <c r="A59" s="46">
         <v>36430</v>
       </c>
-      <c r="B59" s="46">
-        <v>36430</v>
+      <c r="B59" s="124">
+        <v>36343</v>
       </c>
       <c r="C59" s="56">
         <v>38</v>
@@ -47184,8 +47235,8 @@
       <c r="A60" s="46">
         <v>36449</v>
       </c>
-      <c r="B60" s="46">
-        <v>36449</v>
+      <c r="B60" s="124">
+        <v>36347</v>
       </c>
       <c r="C60" s="56">
         <v>38</v>
@@ -47226,8 +47277,8 @@
       <c r="A61" s="46">
         <v>36454</v>
       </c>
-      <c r="B61" s="46">
-        <v>36454</v>
+      <c r="B61" s="124">
+        <v>36350</v>
       </c>
       <c r="C61" s="56">
         <v>32</v>
@@ -47268,8 +47319,8 @@
       <c r="A62" s="46">
         <v>36468</v>
       </c>
-      <c r="B62" s="46">
-        <v>36468</v>
+      <c r="B62" s="124">
+        <v>36352</v>
       </c>
       <c r="C62" s="56">
         <v>32</v>
@@ -47310,8 +47361,8 @@
       <c r="A63" s="46">
         <v>36493</v>
       </c>
-      <c r="B63" s="46">
-        <v>36493</v>
+      <c r="B63" s="124">
+        <v>36360</v>
       </c>
       <c r="C63" s="56">
         <v>32</v>
@@ -47352,8 +47403,8 @@
       <c r="A64" s="46">
         <v>36503</v>
       </c>
-      <c r="B64" s="46">
-        <v>36503</v>
+      <c r="B64" s="124">
+        <v>36364</v>
       </c>
       <c r="C64" s="56">
         <v>32</v>
@@ -47394,8 +47445,8 @@
       <c r="A65" s="46">
         <v>36512</v>
       </c>
-      <c r="B65" s="46">
-        <v>36512</v>
+      <c r="B65" s="124">
+        <v>36368</v>
       </c>
       <c r="C65" s="56">
         <v>32</v>
@@ -47436,8 +47487,8 @@
       <c r="A66" s="46">
         <v>36516</v>
       </c>
-      <c r="B66" s="46">
-        <v>36516</v>
+      <c r="B66" s="124">
+        <v>36370</v>
       </c>
       <c r="C66" s="56">
         <v>32</v>
@@ -47478,8 +47529,8 @@
       <c r="A67" s="46">
         <v>36527</v>
       </c>
-      <c r="B67" s="46">
-        <v>36527</v>
+      <c r="B67" s="124">
+        <v>36381</v>
       </c>
       <c r="C67" s="56">
         <v>32</v>
@@ -47520,8 +47571,8 @@
       <c r="A68" s="46">
         <v>36586</v>
       </c>
-      <c r="B68" s="46">
-        <v>36586</v>
+      <c r="B68" s="124">
+        <v>36385</v>
       </c>
       <c r="C68" s="56">
         <v>32</v>
@@ -47562,8 +47613,8 @@
       <c r="A69" s="46">
         <v>36596</v>
       </c>
-      <c r="B69" s="46">
-        <v>36596</v>
+      <c r="B69" s="124">
+        <v>36390</v>
       </c>
       <c r="C69" s="56">
         <v>32</v>
@@ -47604,8 +47655,8 @@
       <c r="A70" s="46">
         <v>36614</v>
       </c>
-      <c r="B70" s="46">
-        <v>36614</v>
+      <c r="B70" s="124">
+        <v>36394</v>
       </c>
       <c r="C70" s="56">
         <v>32</v>
@@ -47646,8 +47697,8 @@
       <c r="A71" s="46">
         <v>36623</v>
       </c>
-      <c r="B71" s="46">
-        <v>36623</v>
+      <c r="B71" s="124">
+        <v>36407</v>
       </c>
       <c r="C71" s="56">
         <v>32</v>
@@ -47688,8 +47739,8 @@
       <c r="A72" s="46">
         <v>36664</v>
       </c>
-      <c r="B72" s="46">
-        <v>36664</v>
+      <c r="B72" s="124">
+        <v>36413</v>
       </c>
       <c r="C72" s="56">
         <v>32</v>
@@ -47730,8 +47781,8 @@
       <c r="A73" s="46">
         <v>36676</v>
       </c>
-      <c r="B73" s="46">
-        <v>36676</v>
+      <c r="B73" s="124">
+        <v>36420</v>
       </c>
       <c r="C73" s="56">
         <v>36</v>
@@ -47772,8 +47823,8 @@
       <c r="A74" s="46">
         <v>36685</v>
       </c>
-      <c r="B74" s="46">
-        <v>36685</v>
+      <c r="B74" s="124">
+        <v>36428</v>
       </c>
       <c r="C74" s="56">
         <v>36</v>
@@ -47814,8 +47865,8 @@
       <c r="A75" s="46">
         <v>36703</v>
       </c>
-      <c r="B75" s="46">
-        <v>36703</v>
+      <c r="B75" s="124">
+        <v>36433</v>
       </c>
       <c r="C75" s="56">
         <v>25</v>
@@ -47854,8 +47905,8 @@
       <c r="A76" s="46">
         <v>36712</v>
       </c>
-      <c r="B76" s="46">
-        <v>36712</v>
+      <c r="B76" s="124">
+        <v>36439</v>
       </c>
       <c r="C76" s="56">
         <v>25</v>
@@ -47896,8 +47947,8 @@
       <c r="A77" s="46">
         <v>36733</v>
       </c>
-      <c r="B77" s="46">
-        <v>36733</v>
+      <c r="B77" s="124">
+        <v>36444</v>
       </c>
       <c r="C77" s="56">
         <v>25</v>
@@ -47938,8 +47989,8 @@
       <c r="A78" s="46">
         <v>36757</v>
       </c>
-      <c r="B78" s="46">
-        <v>36757</v>
+      <c r="B78" s="124">
+        <v>36456</v>
       </c>
       <c r="C78" s="56">
         <v>25</v>
@@ -47980,8 +48031,8 @@
       <c r="A79" s="46">
         <v>36766</v>
       </c>
-      <c r="B79" s="46">
-        <v>36766</v>
+      <c r="B79" s="124">
+        <v>36460</v>
       </c>
       <c r="C79" s="56">
         <v>25</v>
@@ -48020,8 +48071,8 @@
       <c r="A80" s="46">
         <v>36778</v>
       </c>
-      <c r="B80" s="46">
-        <v>36778</v>
+      <c r="B80" s="124">
+        <v>36474</v>
       </c>
       <c r="C80" s="56">
         <v>25</v>
@@ -48062,8 +48113,8 @@
       <c r="A81" s="46">
         <v>36781</v>
       </c>
-      <c r="B81" s="46">
-        <v>36781</v>
+      <c r="B81" s="124">
+        <v>36505</v>
       </c>
       <c r="C81" s="56">
         <v>25</v>
@@ -48104,8 +48155,8 @@
       <c r="A82" s="46">
         <v>36784</v>
       </c>
-      <c r="B82" s="46">
-        <v>36784</v>
+      <c r="B82" s="124">
+        <v>36513</v>
       </c>
       <c r="C82" s="56">
         <v>25</v>
@@ -48146,8 +48197,8 @@
       <c r="A83" s="46">
         <v>36798</v>
       </c>
-      <c r="B83" s="46">
-        <v>36798</v>
+      <c r="B83" s="124">
+        <v>36519</v>
       </c>
       <c r="C83" s="56">
         <v>25</v>
@@ -48183,8 +48234,8 @@
       <c r="A84" s="46">
         <v>36812</v>
       </c>
-      <c r="B84" s="46">
-        <v>36812</v>
+      <c r="B84" s="124">
+        <v>36531</v>
       </c>
       <c r="C84" s="56">
         <v>14</v>
@@ -48225,8 +48276,8 @@
       <c r="A85" s="46">
         <v>36827</v>
       </c>
-      <c r="B85" s="46">
-        <v>36827</v>
+      <c r="B85" s="124">
+        <v>36536</v>
       </c>
       <c r="C85" s="56">
         <v>14</v>
@@ -48267,8 +48318,8 @@
       <c r="A86" s="46">
         <v>36835</v>
       </c>
-      <c r="B86" s="46">
-        <v>36835</v>
+      <c r="B86" s="124">
+        <v>36548</v>
       </c>
       <c r="C86" s="56">
         <v>20</v>
@@ -48309,8 +48360,8 @@
       <c r="A87" s="46">
         <v>36860</v>
       </c>
-      <c r="B87" s="46">
-        <v>36860</v>
+      <c r="B87" s="124">
+        <v>36556</v>
       </c>
       <c r="C87" s="56">
         <v>14</v>
@@ -48349,8 +48400,8 @@
       <c r="A88" s="46">
         <v>36896</v>
       </c>
-      <c r="B88" s="46">
-        <v>36896</v>
+      <c r="B88" s="124">
+        <v>36566</v>
       </c>
       <c r="C88" s="56">
         <v>14</v>
@@ -48391,8 +48442,8 @@
       <c r="A89" s="46">
         <v>36911</v>
       </c>
-      <c r="B89" s="46">
-        <v>36911</v>
+      <c r="B89" s="124">
+        <v>36576</v>
       </c>
       <c r="C89" s="56">
         <v>18</v>
@@ -48433,8 +48484,8 @@
       <c r="A90" s="46">
         <v>36931</v>
       </c>
-      <c r="B90" s="46">
-        <v>36931</v>
+      <c r="B90" s="124">
+        <v>36582</v>
       </c>
       <c r="C90" s="56">
         <v>30</v>
@@ -48475,8 +48526,8 @@
       <c r="A91" s="46">
         <v>36935</v>
       </c>
-      <c r="B91" s="46">
-        <v>36935</v>
+      <c r="B91" s="124">
+        <v>36590</v>
       </c>
       <c r="C91" s="56">
         <v>30</v>
@@ -48517,8 +48568,8 @@
       <c r="A92" s="46">
         <v>36946</v>
       </c>
-      <c r="B92" s="46">
-        <v>36946</v>
+      <c r="B92" s="124">
+        <v>36602</v>
       </c>
       <c r="C92" s="56">
         <v>30</v>
@@ -48559,8 +48610,8 @@
       <c r="A93" s="46">
         <v>36953</v>
       </c>
-      <c r="B93" s="46">
-        <v>36953</v>
+      <c r="B93" s="124">
+        <v>36622</v>
       </c>
       <c r="C93" s="56">
         <v>30</v>
@@ -48601,8 +48652,8 @@
       <c r="A94" s="46">
         <v>36998</v>
       </c>
-      <c r="B94" s="46">
-        <v>36998</v>
+      <c r="B94" s="124">
+        <v>36629</v>
       </c>
       <c r="C94" s="56">
         <v>30</v>
@@ -48643,8 +48694,8 @@
       <c r="A95" s="46">
         <v>37018</v>
       </c>
-      <c r="B95" s="46">
-        <v>37018</v>
+      <c r="B95" s="124">
+        <v>36632</v>
       </c>
       <c r="C95" s="56">
         <v>30</v>
@@ -48685,8 +48736,8 @@
       <c r="A96" s="46">
         <v>37044</v>
       </c>
-      <c r="B96" s="46">
-        <v>37044</v>
+      <c r="B96" s="124">
+        <v>36645</v>
       </c>
       <c r="C96" s="56">
         <v>30</v>
@@ -48727,8 +48778,8 @@
       <c r="A97" s="46">
         <v>37074</v>
       </c>
-      <c r="B97" s="46">
-        <v>37074</v>
+      <c r="B97" s="124">
+        <v>36651</v>
       </c>
       <c r="C97" s="56">
         <v>30</v>
@@ -48770,8 +48821,8 @@
       <c r="A98" s="46">
         <v>37103</v>
       </c>
-      <c r="B98" s="46">
-        <v>37103</v>
+      <c r="B98" s="124">
+        <v>36659</v>
       </c>
       <c r="C98" s="56">
         <v>30</v>
@@ -48813,8 +48864,8 @@
       <c r="A99" s="46">
         <v>37166</v>
       </c>
-      <c r="B99" s="46">
-        <v>37166</v>
+      <c r="B99" s="124">
+        <v>36668</v>
       </c>
       <c r="C99" s="56"/>
       <c r="D99" s="71">
@@ -48854,8 +48905,8 @@
       <c r="A100" s="46">
         <v>37190</v>
       </c>
-      <c r="B100" s="46">
-        <v>37190</v>
+      <c r="B100" s="124">
+        <v>36670</v>
       </c>
       <c r="C100" s="56"/>
       <c r="D100" s="71">
@@ -48895,8 +48946,8 @@
       <c r="A101" s="46">
         <v>37217</v>
       </c>
-      <c r="B101" s="46">
-        <v>37217</v>
+      <c r="B101" s="124">
+        <v>36679</v>
       </c>
       <c r="C101" s="56"/>
       <c r="D101" s="71">
@@ -48936,8 +48987,8 @@
       <c r="A102" s="46">
         <v>37237</v>
       </c>
-      <c r="B102" s="46">
-        <v>37237</v>
+      <c r="B102" s="124">
+        <v>36688</v>
       </c>
       <c r="C102" s="56"/>
       <c r="D102" s="71">
@@ -48977,8 +49028,8 @@
       <c r="A103" s="46">
         <v>37267</v>
       </c>
-      <c r="B103" s="46">
-        <v>37267</v>
+      <c r="B103" s="124">
+        <v>36720</v>
       </c>
       <c r="C103" s="56"/>
       <c r="D103" s="71">
@@ -49018,8 +49069,8 @@
       <c r="A104" s="46">
         <v>37299</v>
       </c>
-      <c r="B104" s="46">
-        <v>37299</v>
+      <c r="B104" s="124">
+        <v>36735</v>
       </c>
       <c r="C104" s="56"/>
       <c r="D104" s="71">
@@ -49059,8 +49110,8 @@
       <c r="A105" s="46">
         <v>37325</v>
       </c>
-      <c r="B105" s="46">
-        <v>37325</v>
+      <c r="B105" s="124">
+        <v>36749</v>
       </c>
       <c r="C105" s="56"/>
       <c r="D105" s="71">
@@ -49100,8 +49151,8 @@
       <c r="A106" s="46">
         <v>37356</v>
       </c>
-      <c r="B106" s="46">
-        <v>37356</v>
+      <c r="B106" s="124">
+        <v>36754</v>
       </c>
       <c r="C106" s="56"/>
       <c r="D106" s="71">
@@ -49141,8 +49192,8 @@
       <c r="A107" s="46">
         <v>37377</v>
       </c>
-      <c r="B107" s="46">
-        <v>37377</v>
+      <c r="B107" s="124">
+        <v>36760</v>
       </c>
       <c r="C107" s="56"/>
       <c r="D107" s="71">
@@ -49182,8 +49233,8 @@
       <c r="A108" s="46">
         <v>37410</v>
       </c>
-      <c r="B108" s="46">
-        <v>37410</v>
+      <c r="B108" s="124">
+        <v>36793</v>
       </c>
       <c r="C108" s="56"/>
       <c r="D108" s="71">
@@ -49218,25 +49269,25 @@
         <v>2016.5244069135204</v>
       </c>
       <c r="M108" s="61"/>
-      <c r="U108" s="115" t="s">
+      <c r="U108" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="V108" s="116"/>
-      <c r="W108" s="116" t="s">
+      <c r="V108" s="84"/>
+      <c r="W108" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="X108" s="116"/>
-      <c r="Y108" s="116" t="s">
+      <c r="X108" s="84"/>
+      <c r="Y108" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="Z108" s="116"/>
+      <c r="Z108" s="84"/>
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" thickTop="1">
       <c r="A109" s="46">
         <v>37438</v>
       </c>
-      <c r="B109" s="46">
-        <v>37438</v>
+      <c r="B109" s="124">
+        <v>36799</v>
       </c>
       <c r="C109" s="56"/>
       <c r="D109" s="71">
@@ -49273,25 +49324,25 @@
       <c r="M109" s="61"/>
       <c r="R109"/>
       <c r="S109" s="73"/>
-      <c r="U109" s="117" t="s">
+      <c r="U109" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="V109" s="122"/>
-      <c r="W109" s="117" t="s">
+      <c r="V109" s="86"/>
+      <c r="W109" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="X109" s="122"/>
-      <c r="Y109" s="118" t="s">
+      <c r="X109" s="86"/>
+      <c r="Y109" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="Z109" s="118"/>
+      <c r="Z109" s="87"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1">
       <c r="A110" s="46">
         <v>37468</v>
       </c>
-      <c r="B110" s="46">
-        <v>37468</v>
+      <c r="B110" s="124">
+        <v>36808</v>
       </c>
       <c r="C110" s="56"/>
       <c r="D110" s="71">
@@ -49328,25 +49379,25 @@
       <c r="M110" s="61"/>
       <c r="R110"/>
       <c r="S110" s="74"/>
-      <c r="U110" s="119" t="s">
+      <c r="U110" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="V110" s="119"/>
-      <c r="W110" s="119" t="s">
+      <c r="V110" s="88"/>
+      <c r="W110" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="X110" s="119"/>
-      <c r="Y110" s="119" t="s">
+      <c r="X110" s="88"/>
+      <c r="Y110" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="Z110" s="119"/>
+      <c r="Z110" s="88"/>
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1">
       <c r="A111" s="46">
         <v>37504</v>
       </c>
-      <c r="B111" s="46">
-        <v>37504</v>
+      <c r="B111" s="124">
+        <v>36824</v>
       </c>
       <c r="C111" s="56"/>
       <c r="D111" s="71">
@@ -49383,25 +49434,25 @@
       <c r="M111" s="61"/>
       <c r="R111"/>
       <c r="S111" s="75"/>
-      <c r="U111" s="94" t="s">
+      <c r="U111" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="V111" s="94"/>
-      <c r="W111" s="94" t="s">
+      <c r="V111" s="108"/>
+      <c r="W111" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="X111" s="94"/>
-      <c r="Y111" s="94" t="s">
+      <c r="X111" s="108"/>
+      <c r="Y111" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="Z111" s="94"/>
+      <c r="Z111" s="108"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1">
       <c r="A112" s="46">
         <v>37517</v>
       </c>
-      <c r="B112" s="46">
-        <v>37517</v>
+      <c r="B112" s="124">
+        <v>36843</v>
       </c>
       <c r="C112" s="56"/>
       <c r="D112" s="71">
@@ -49438,25 +49489,25 @@
       <c r="M112" s="61"/>
       <c r="R112"/>
       <c r="S112" s="75"/>
-      <c r="U112" s="96" t="s">
+      <c r="U112" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="V112" s="96"/>
-      <c r="W112" s="96" t="s">
+      <c r="V112" s="110"/>
+      <c r="W112" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="X112" s="96"/>
-      <c r="Y112" s="96" t="s">
+      <c r="X112" s="110"/>
+      <c r="Y112" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="Z112" s="96"/>
+      <c r="Z112" s="110"/>
     </row>
     <row r="113" spans="1:29" ht="16.5" thickBot="1">
       <c r="A113" s="46">
         <v>37531</v>
       </c>
-      <c r="B113" s="46">
-        <v>37531</v>
+      <c r="B113" s="124">
+        <v>36845</v>
       </c>
       <c r="C113" s="56"/>
       <c r="D113" s="70">
@@ -49493,25 +49544,25 @@
       <c r="M113" s="61"/>
       <c r="R113"/>
       <c r="S113" s="75"/>
-      <c r="U113" s="97" t="s">
+      <c r="U113" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="V113" s="98"/>
-      <c r="W113" s="97" t="s">
+      <c r="V113" s="112"/>
+      <c r="W113" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="X113" s="98"/>
-      <c r="Y113" s="98" t="s">
+      <c r="X113" s="112"/>
+      <c r="Y113" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="Z113" s="98"/>
+      <c r="Z113" s="112"/>
     </row>
     <row r="114" spans="1:29" ht="16.5" customHeight="1" thickBot="1">
       <c r="A114" s="46">
         <v>37566</v>
       </c>
-      <c r="B114" s="46">
-        <v>37566</v>
+      <c r="B114" s="124">
+        <v>36857</v>
       </c>
       <c r="C114" s="56"/>
       <c r="D114" s="71">
@@ -49555,8 +49606,8 @@
       <c r="A115" s="46">
         <v>37594</v>
       </c>
-      <c r="B115" s="46">
-        <v>37594</v>
+      <c r="B115" s="124">
+        <v>36887</v>
       </c>
       <c r="C115" s="56"/>
       <c r="D115" s="71">
@@ -49591,29 +49642,29 @@
         <v>2043.9609368042982</v>
       </c>
       <c r="M115" s="61"/>
-      <c r="R115" s="102" t="s">
+      <c r="R115" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="S115" s="102"/>
-      <c r="T115" s="102"/>
-      <c r="U115" s="102"/>
-      <c r="V115" s="102"/>
-      <c r="W115" s="102"/>
-      <c r="X115" s="102"/>
-      <c r="Y115" s="102"/>
-      <c r="Z115" s="102"/>
-      <c r="AA115" s="105" t="s">
+      <c r="S115" s="99"/>
+      <c r="T115" s="99"/>
+      <c r="U115" s="99"/>
+      <c r="V115" s="99"/>
+      <c r="W115" s="99"/>
+      <c r="X115" s="99"/>
+      <c r="Y115" s="99"/>
+      <c r="Z115" s="99"/>
+      <c r="AA115" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="AB115" s="105"/>
-      <c r="AC115" s="105"/>
+      <c r="AB115" s="102"/>
+      <c r="AC115" s="102"/>
     </row>
     <row r="116" spans="1:29" ht="15.75" customHeight="1">
       <c r="A116" s="46">
         <v>37628</v>
       </c>
-      <c r="B116" s="46">
-        <v>37628</v>
+      <c r="B116" s="124">
+        <v>36902</v>
       </c>
       <c r="C116" s="56"/>
       <c r="D116" s="71">
@@ -49648,25 +49699,25 @@
         <v>2062.9866810979825</v>
       </c>
       <c r="M116" s="61"/>
-      <c r="R116" s="103"/>
-      <c r="S116" s="103"/>
-      <c r="T116" s="103"/>
-      <c r="U116" s="103"/>
-      <c r="V116" s="103"/>
-      <c r="W116" s="103"/>
-      <c r="X116" s="103"/>
-      <c r="Y116" s="103"/>
-      <c r="Z116" s="103"/>
-      <c r="AA116" s="106"/>
-      <c r="AB116" s="106"/>
-      <c r="AC116" s="106"/>
+      <c r="R116" s="100"/>
+      <c r="S116" s="100"/>
+      <c r="T116" s="100"/>
+      <c r="U116" s="100"/>
+      <c r="V116" s="100"/>
+      <c r="W116" s="100"/>
+      <c r="X116" s="100"/>
+      <c r="Y116" s="100"/>
+      <c r="Z116" s="100"/>
+      <c r="AA116" s="103"/>
+      <c r="AB116" s="103"/>
+      <c r="AC116" s="103"/>
     </row>
     <row r="117" spans="1:29" ht="15.75" customHeight="1">
       <c r="A117" s="46">
         <v>37657</v>
       </c>
-      <c r="B117" s="46">
-        <v>37657</v>
+      <c r="B117" s="124">
+        <v>36909</v>
       </c>
       <c r="C117" s="56"/>
       <c r="D117" s="71"/>
@@ -49699,25 +49750,25 @@
         <v>1964.8104553941066</v>
       </c>
       <c r="M117" s="61"/>
-      <c r="R117" s="103"/>
-      <c r="S117" s="103"/>
-      <c r="T117" s="103"/>
-      <c r="U117" s="103"/>
-      <c r="V117" s="103"/>
-      <c r="W117" s="103"/>
-      <c r="X117" s="103"/>
-      <c r="Y117" s="103"/>
-      <c r="Z117" s="103"/>
-      <c r="AA117" s="106"/>
-      <c r="AB117" s="106"/>
-      <c r="AC117" s="106"/>
+      <c r="R117" s="100"/>
+      <c r="S117" s="100"/>
+      <c r="T117" s="100"/>
+      <c r="U117" s="100"/>
+      <c r="V117" s="100"/>
+      <c r="W117" s="100"/>
+      <c r="X117" s="100"/>
+      <c r="Y117" s="100"/>
+      <c r="Z117" s="100"/>
+      <c r="AA117" s="103"/>
+      <c r="AB117" s="103"/>
+      <c r="AC117" s="103"/>
     </row>
     <row r="118" spans="1:29" ht="15.75" customHeight="1">
       <c r="A118" s="46">
         <v>37685</v>
       </c>
-      <c r="B118" s="46">
-        <v>37685</v>
+      <c r="B118" s="124">
+        <v>36933</v>
       </c>
       <c r="C118" s="56"/>
       <c r="D118" s="71">
@@ -49752,25 +49803,25 @@
         <v>1723.6846830669779</v>
       </c>
       <c r="M118" s="61"/>
-      <c r="R118" s="103"/>
-      <c r="S118" s="103"/>
-      <c r="T118" s="103"/>
-      <c r="U118" s="103"/>
-      <c r="V118" s="103"/>
-      <c r="W118" s="103"/>
-      <c r="X118" s="103"/>
-      <c r="Y118" s="103"/>
-      <c r="Z118" s="103"/>
-      <c r="AA118" s="106"/>
-      <c r="AB118" s="106"/>
-      <c r="AC118" s="106"/>
+      <c r="R118" s="100"/>
+      <c r="S118" s="100"/>
+      <c r="T118" s="100"/>
+      <c r="U118" s="100"/>
+      <c r="V118" s="100"/>
+      <c r="W118" s="100"/>
+      <c r="X118" s="100"/>
+      <c r="Y118" s="100"/>
+      <c r="Z118" s="100"/>
+      <c r="AA118" s="103"/>
+      <c r="AB118" s="103"/>
+      <c r="AC118" s="103"/>
     </row>
     <row r="119" spans="1:29" ht="15.75" customHeight="1">
       <c r="A119" s="46">
         <v>37714</v>
       </c>
-      <c r="B119" s="46">
-        <v>37714</v>
+      <c r="B119" s="124">
+        <v>36935</v>
       </c>
       <c r="C119" s="56"/>
       <c r="D119" s="71">
@@ -49805,25 +49856,25 @@
         <v>1556.6508313539193</v>
       </c>
       <c r="M119" s="61"/>
-      <c r="R119" s="103"/>
-      <c r="S119" s="103"/>
-      <c r="T119" s="103"/>
-      <c r="U119" s="103"/>
-      <c r="V119" s="103"/>
-      <c r="W119" s="103"/>
-      <c r="X119" s="103"/>
-      <c r="Y119" s="103"/>
-      <c r="Z119" s="103"/>
-      <c r="AA119" s="106"/>
-      <c r="AB119" s="106"/>
-      <c r="AC119" s="106"/>
+      <c r="R119" s="100"/>
+      <c r="S119" s="100"/>
+      <c r="T119" s="100"/>
+      <c r="U119" s="100"/>
+      <c r="V119" s="100"/>
+      <c r="W119" s="100"/>
+      <c r="X119" s="100"/>
+      <c r="Y119" s="100"/>
+      <c r="Z119" s="100"/>
+      <c r="AA119" s="103"/>
+      <c r="AB119" s="103"/>
+      <c r="AC119" s="103"/>
     </row>
     <row r="120" spans="1:29" ht="15.75" customHeight="1">
       <c r="A120" s="46">
         <v>37750</v>
       </c>
-      <c r="B120" s="46">
-        <v>37750</v>
+      <c r="B120" s="124">
+        <v>36948</v>
       </c>
       <c r="C120" s="56"/>
       <c r="D120" s="71">
@@ -49858,25 +49909,25 @@
         <v>1653.9242483404919</v>
       </c>
       <c r="M120" s="61"/>
-      <c r="R120" s="103"/>
-      <c r="S120" s="103"/>
-      <c r="T120" s="103"/>
-      <c r="U120" s="103"/>
-      <c r="V120" s="103"/>
-      <c r="W120" s="103"/>
-      <c r="X120" s="103"/>
-      <c r="Y120" s="103"/>
-      <c r="Z120" s="103"/>
-      <c r="AA120" s="106"/>
-      <c r="AB120" s="106"/>
-      <c r="AC120" s="106"/>
+      <c r="R120" s="100"/>
+      <c r="S120" s="100"/>
+      <c r="T120" s="100"/>
+      <c r="U120" s="100"/>
+      <c r="V120" s="100"/>
+      <c r="W120" s="100"/>
+      <c r="X120" s="100"/>
+      <c r="Y120" s="100"/>
+      <c r="Z120" s="100"/>
+      <c r="AA120" s="103"/>
+      <c r="AB120" s="103"/>
+      <c r="AC120" s="103"/>
     </row>
     <row r="121" spans="1:29" ht="15.75" customHeight="1">
       <c r="A121" s="46">
         <v>37783</v>
       </c>
-      <c r="B121" s="46">
-        <v>37783</v>
+      <c r="B121" s="124">
+        <v>36949</v>
       </c>
       <c r="C121" s="56"/>
       <c r="D121" s="71">
@@ -49911,25 +49962,25 @@
         <v>1675.9837374764047</v>
       </c>
       <c r="M121" s="61"/>
-      <c r="R121" s="103"/>
-      <c r="S121" s="103"/>
-      <c r="T121" s="103"/>
-      <c r="U121" s="103"/>
-      <c r="V121" s="103"/>
-      <c r="W121" s="103"/>
-      <c r="X121" s="103"/>
-      <c r="Y121" s="103"/>
-      <c r="Z121" s="103"/>
-      <c r="AA121" s="106"/>
-      <c r="AB121" s="106"/>
-      <c r="AC121" s="106"/>
+      <c r="R121" s="100"/>
+      <c r="S121" s="100"/>
+      <c r="T121" s="100"/>
+      <c r="U121" s="100"/>
+      <c r="V121" s="100"/>
+      <c r="W121" s="100"/>
+      <c r="X121" s="100"/>
+      <c r="Y121" s="100"/>
+      <c r="Z121" s="100"/>
+      <c r="AA121" s="103"/>
+      <c r="AB121" s="103"/>
+      <c r="AC121" s="103"/>
     </row>
     <row r="122" spans="1:29" ht="18" customHeight="1">
       <c r="A122" s="46">
         <v>37816</v>
       </c>
-      <c r="B122" s="46">
-        <v>37816</v>
+      <c r="B122" s="124">
+        <v>36963</v>
       </c>
       <c r="C122" s="56"/>
       <c r="D122" s="71">
@@ -49963,25 +50014,25 @@
         <v>1329.8016843249118</v>
       </c>
       <c r="M122" s="61"/>
-      <c r="R122" s="104"/>
-      <c r="S122" s="104"/>
-      <c r="T122" s="104"/>
-      <c r="U122" s="104"/>
-      <c r="V122" s="104"/>
-      <c r="W122" s="104"/>
-      <c r="X122" s="104"/>
-      <c r="Y122" s="104"/>
-      <c r="Z122" s="104"/>
-      <c r="AA122" s="107"/>
-      <c r="AB122" s="107"/>
-      <c r="AC122" s="107"/>
+      <c r="R122" s="101"/>
+      <c r="S122" s="101"/>
+      <c r="T122" s="101"/>
+      <c r="U122" s="101"/>
+      <c r="V122" s="101"/>
+      <c r="W122" s="101"/>
+      <c r="X122" s="101"/>
+      <c r="Y122" s="101"/>
+      <c r="Z122" s="101"/>
+      <c r="AA122" s="104"/>
+      <c r="AB122" s="104"/>
+      <c r="AC122" s="104"/>
     </row>
     <row r="123" spans="1:29" ht="16.5" customHeight="1" thickBot="1">
       <c r="A123" s="46">
         <v>37852</v>
       </c>
-      <c r="B123" s="46">
-        <v>37852</v>
+      <c r="B123" s="124">
+        <v>36970</v>
       </c>
       <c r="C123" s="56"/>
       <c r="D123" s="71">
@@ -50015,27 +50066,27 @@
         <v>1677.1060078363082</v>
       </c>
       <c r="M123" s="61"/>
-      <c r="R123" s="100"/>
-      <c r="S123" s="100"/>
-      <c r="T123" s="100"/>
-      <c r="U123" s="100"/>
-      <c r="V123" s="100"/>
-      <c r="W123" s="100"/>
-      <c r="X123" s="100"/>
-      <c r="Y123" s="100"/>
-      <c r="Z123" s="100"/>
-      <c r="AA123" s="101" t="s">
+      <c r="R123" s="97"/>
+      <c r="S123" s="97"/>
+      <c r="T123" s="97"/>
+      <c r="U123" s="97"/>
+      <c r="V123" s="97"/>
+      <c r="W123" s="97"/>
+      <c r="X123" s="97"/>
+      <c r="Y123" s="97"/>
+      <c r="Z123" s="97"/>
+      <c r="AA123" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="AB123" s="101"/>
-      <c r="AC123" s="101"/>
+      <c r="AB123" s="98"/>
+      <c r="AC123" s="98"/>
     </row>
     <row r="124" spans="1:29" ht="15.75" customHeight="1" thickTop="1">
       <c r="A124" s="46">
         <v>37883</v>
       </c>
-      <c r="B124" s="46">
-        <v>37883</v>
+      <c r="B124" s="124">
+        <v>36972</v>
       </c>
       <c r="C124" s="56"/>
       <c r="D124" s="71">
@@ -50069,29 +50120,29 @@
         <v>1574.3356661415696</v>
       </c>
       <c r="M124" s="61"/>
-      <c r="R124" s="108" t="s">
+      <c r="R124" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="S124" s="108"/>
-      <c r="T124" s="108"/>
-      <c r="U124" s="108"/>
-      <c r="V124" s="108"/>
-      <c r="W124" s="108"/>
-      <c r="X124" s="108"/>
-      <c r="Y124" s="108"/>
-      <c r="Z124" s="108"/>
-      <c r="AA124" s="87" t="s">
+      <c r="S124" s="105"/>
+      <c r="T124" s="105"/>
+      <c r="U124" s="105"/>
+      <c r="V124" s="105"/>
+      <c r="W124" s="105"/>
+      <c r="X124" s="105"/>
+      <c r="Y124" s="105"/>
+      <c r="Z124" s="105"/>
+      <c r="AA124" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="AB124" s="87"/>
-      <c r="AC124" s="87"/>
+      <c r="AB124" s="106"/>
+      <c r="AC124" s="106"/>
     </row>
     <row r="125" spans="1:29" ht="15.75" customHeight="1">
       <c r="A125" s="46">
         <v>37924</v>
       </c>
-      <c r="B125" s="46">
-        <v>37924</v>
+      <c r="B125" s="124">
+        <v>37004</v>
       </c>
       <c r="C125" s="56"/>
       <c r="D125" s="71">
@@ -50125,25 +50176,25 @@
         <v>1607.3788693581614</v>
       </c>
       <c r="M125" s="61"/>
-      <c r="R125" s="103"/>
-      <c r="S125" s="103"/>
-      <c r="T125" s="103"/>
-      <c r="U125" s="103"/>
-      <c r="V125" s="103"/>
-      <c r="W125" s="103"/>
-      <c r="X125" s="103"/>
-      <c r="Y125" s="103"/>
-      <c r="Z125" s="103"/>
-      <c r="AA125" s="88"/>
-      <c r="AB125" s="88"/>
-      <c r="AC125" s="88"/>
+      <c r="R125" s="100"/>
+      <c r="S125" s="100"/>
+      <c r="T125" s="100"/>
+      <c r="U125" s="100"/>
+      <c r="V125" s="100"/>
+      <c r="W125" s="100"/>
+      <c r="X125" s="100"/>
+      <c r="Y125" s="100"/>
+      <c r="Z125" s="100"/>
+      <c r="AA125" s="107"/>
+      <c r="AB125" s="107"/>
+      <c r="AC125" s="107"/>
     </row>
     <row r="126" spans="1:29" ht="15.75" customHeight="1">
       <c r="A126" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B126" s="46">
-        <v>37984</v>
+      <c r="B126" s="124">
+        <v>37019</v>
       </c>
       <c r="C126" s="56"/>
       <c r="D126" s="71">
@@ -50177,25 +50228,25 @@
         <v>1601.727170118382</v>
       </c>
       <c r="M126" s="61"/>
-      <c r="R126" s="103"/>
-      <c r="S126" s="103"/>
-      <c r="T126" s="103"/>
-      <c r="U126" s="103"/>
-      <c r="V126" s="103"/>
-      <c r="W126" s="103"/>
-      <c r="X126" s="103"/>
-      <c r="Y126" s="103"/>
-      <c r="Z126" s="103"/>
-      <c r="AA126" s="88"/>
-      <c r="AB126" s="88"/>
-      <c r="AC126" s="88"/>
+      <c r="R126" s="100"/>
+      <c r="S126" s="100"/>
+      <c r="T126" s="100"/>
+      <c r="U126" s="100"/>
+      <c r="V126" s="100"/>
+      <c r="W126" s="100"/>
+      <c r="X126" s="100"/>
+      <c r="Y126" s="100"/>
+      <c r="Z126" s="100"/>
+      <c r="AA126" s="107"/>
+      <c r="AB126" s="107"/>
+      <c r="AC126" s="107"/>
     </row>
     <row r="127" spans="1:29" ht="21.75" customHeight="1">
       <c r="A127" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="B127" s="46">
-        <v>38017</v>
+      <c r="B127" s="124">
+        <v>37045</v>
       </c>
       <c r="C127" s="56"/>
       <c r="D127" s="71">
@@ -50229,25 +50280,25 @@
         <v>1578.1633826373281</v>
       </c>
       <c r="M127" s="61"/>
-      <c r="R127" s="103"/>
-      <c r="S127" s="103"/>
-      <c r="T127" s="103"/>
-      <c r="U127" s="103"/>
-      <c r="V127" s="103"/>
-      <c r="W127" s="103"/>
-      <c r="X127" s="103"/>
-      <c r="Y127" s="103"/>
-      <c r="Z127" s="103"/>
-      <c r="AA127" s="88"/>
-      <c r="AB127" s="88"/>
-      <c r="AC127" s="88"/>
+      <c r="R127" s="100"/>
+      <c r="S127" s="100"/>
+      <c r="T127" s="100"/>
+      <c r="U127" s="100"/>
+      <c r="V127" s="100"/>
+      <c r="W127" s="100"/>
+      <c r="X127" s="100"/>
+      <c r="Y127" s="100"/>
+      <c r="Z127" s="100"/>
+      <c r="AA127" s="107"/>
+      <c r="AB127" s="107"/>
+      <c r="AC127" s="107"/>
     </row>
     <row r="128" spans="1:29" ht="15.75" customHeight="1" thickBot="1">
       <c r="A128" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="B128" s="46">
-        <v>38047</v>
+      <c r="B128" s="124">
+        <v>37073</v>
       </c>
       <c r="C128" s="56"/>
       <c r="D128" s="71">
@@ -50281,27 +50332,27 @@
         <v>1535.3782407274191</v>
       </c>
       <c r="M128" s="61"/>
-      <c r="R128" s="95"/>
-      <c r="S128" s="95"/>
-      <c r="T128" s="95"/>
-      <c r="U128" s="95"/>
-      <c r="V128" s="95"/>
-      <c r="W128" s="95"/>
-      <c r="X128" s="95"/>
-      <c r="Y128" s="95"/>
-      <c r="Z128" s="95"/>
-      <c r="AA128" s="99" t="s">
+      <c r="R128" s="109"/>
+      <c r="S128" s="109"/>
+      <c r="T128" s="109"/>
+      <c r="U128" s="109"/>
+      <c r="V128" s="109"/>
+      <c r="W128" s="109"/>
+      <c r="X128" s="109"/>
+      <c r="Y128" s="109"/>
+      <c r="Z128" s="109"/>
+      <c r="AA128" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="AB128" s="99"/>
-      <c r="AC128" s="99"/>
+      <c r="AB128" s="96"/>
+      <c r="AC128" s="96"/>
     </row>
     <row r="129" spans="1:29" ht="16.5" customHeight="1" thickTop="1">
       <c r="A129" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B129" s="46">
-        <v>38076</v>
+      <c r="B129" s="124">
+        <v>37104</v>
       </c>
       <c r="C129" s="56"/>
       <c r="D129" s="71">
@@ -50335,29 +50386,29 @@
         <v>1513.7643769277336</v>
       </c>
       <c r="M129" s="61"/>
-      <c r="R129" s="84" t="s">
+      <c r="R129" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="S129" s="84"/>
-      <c r="T129" s="84"/>
-      <c r="U129" s="84"/>
-      <c r="V129" s="84"/>
-      <c r="W129" s="84"/>
-      <c r="X129" s="84"/>
-      <c r="Y129" s="84"/>
-      <c r="Z129" s="84"/>
-      <c r="AA129" s="87" t="s">
+      <c r="S129" s="113"/>
+      <c r="T129" s="113"/>
+      <c r="U129" s="113"/>
+      <c r="V129" s="113"/>
+      <c r="W129" s="113"/>
+      <c r="X129" s="113"/>
+      <c r="Y129" s="113"/>
+      <c r="Z129" s="113"/>
+      <c r="AA129" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="AB129" s="87"/>
-      <c r="AC129" s="87"/>
+      <c r="AB129" s="106"/>
+      <c r="AC129" s="106"/>
     </row>
     <row r="130" spans="1:29">
       <c r="A130" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B130" s="46">
-        <v>38106</v>
+      <c r="B130" s="124">
+        <v>37167</v>
       </c>
       <c r="C130" s="56"/>
       <c r="D130" s="71">
@@ -50391,25 +50442,25 @@
         <v>1485.1259916005599</v>
       </c>
       <c r="M130" s="61"/>
-      <c r="R130" s="85"/>
-      <c r="S130" s="85"/>
-      <c r="T130" s="85"/>
-      <c r="U130" s="85"/>
-      <c r="V130" s="85"/>
-      <c r="W130" s="85"/>
-      <c r="X130" s="85"/>
-      <c r="Y130" s="85"/>
-      <c r="Z130" s="85"/>
-      <c r="AA130" s="88"/>
-      <c r="AB130" s="88"/>
-      <c r="AC130" s="88"/>
+      <c r="R130" s="114"/>
+      <c r="S130" s="114"/>
+      <c r="T130" s="114"/>
+      <c r="U130" s="114"/>
+      <c r="V130" s="114"/>
+      <c r="W130" s="114"/>
+      <c r="X130" s="114"/>
+      <c r="Y130" s="114"/>
+      <c r="Z130" s="114"/>
+      <c r="AA130" s="107"/>
+      <c r="AB130" s="107"/>
+      <c r="AC130" s="107"/>
     </row>
     <row r="131" spans="1:29">
       <c r="A131" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B131" s="46">
-        <v>38138</v>
+      <c r="B131" s="124">
+        <v>37187</v>
       </c>
       <c r="C131" s="56"/>
       <c r="D131" s="71">
@@ -50443,25 +50494,25 @@
         <v>1484.0190763944429</v>
       </c>
       <c r="M131" s="61"/>
-      <c r="R131" s="86"/>
-      <c r="S131" s="86"/>
-      <c r="T131" s="86"/>
-      <c r="U131" s="86"/>
-      <c r="V131" s="86"/>
-      <c r="W131" s="86"/>
-      <c r="X131" s="86"/>
-      <c r="Y131" s="86"/>
-      <c r="Z131" s="86"/>
-      <c r="AA131" s="89"/>
-      <c r="AB131" s="89"/>
-      <c r="AC131" s="89"/>
+      <c r="R131" s="115"/>
+      <c r="S131" s="115"/>
+      <c r="T131" s="115"/>
+      <c r="U131" s="115"/>
+      <c r="V131" s="115"/>
+      <c r="W131" s="115"/>
+      <c r="X131" s="115"/>
+      <c r="Y131" s="115"/>
+      <c r="Z131" s="115"/>
+      <c r="AA131" s="116"/>
+      <c r="AB131" s="116"/>
+      <c r="AC131" s="116"/>
     </row>
     <row r="132" spans="1:29">
       <c r="A132" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="B132" s="46">
-        <v>38171</v>
+      <c r="B132" s="124">
+        <v>37194</v>
       </c>
       <c r="C132" s="56"/>
       <c r="D132" s="71">
@@ -50495,27 +50546,27 @@
         <v>1824.7824674152437</v>
       </c>
       <c r="M132" s="61"/>
-      <c r="R132" s="90"/>
-      <c r="S132" s="90"/>
-      <c r="T132" s="90"/>
-      <c r="U132" s="90"/>
-      <c r="V132" s="90"/>
-      <c r="W132" s="90"/>
-      <c r="X132" s="90"/>
-      <c r="Y132" s="90"/>
-      <c r="Z132" s="90"/>
-      <c r="AA132" s="91" t="s">
+      <c r="R132" s="117"/>
+      <c r="S132" s="117"/>
+      <c r="T132" s="117"/>
+      <c r="U132" s="117"/>
+      <c r="V132" s="117"/>
+      <c r="W132" s="117"/>
+      <c r="X132" s="117"/>
+      <c r="Y132" s="117"/>
+      <c r="Z132" s="117"/>
+      <c r="AA132" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="AB132" s="91"/>
-      <c r="AC132" s="91"/>
+      <c r="AB132" s="118"/>
+      <c r="AC132" s="118"/>
     </row>
     <row r="133" spans="1:29" ht="16.5" thickBot="1">
       <c r="A133" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="B133" s="46">
-        <v>38213</v>
+      <c r="B133" s="124">
+        <v>37220</v>
       </c>
       <c r="C133" s="56"/>
       <c r="D133" s="71">
@@ -50549,27 +50600,27 @@
         <v>1331.3515954244431</v>
       </c>
       <c r="M133" s="61"/>
-      <c r="R133" s="92"/>
-      <c r="S133" s="92"/>
-      <c r="T133" s="92"/>
-      <c r="U133" s="92"/>
-      <c r="V133" s="92"/>
-      <c r="W133" s="92"/>
-      <c r="X133" s="92"/>
-      <c r="Y133" s="92"/>
-      <c r="Z133" s="92"/>
-      <c r="AA133" s="93" t="s">
+      <c r="R133" s="119"/>
+      <c r="S133" s="119"/>
+      <c r="T133" s="119"/>
+      <c r="U133" s="119"/>
+      <c r="V133" s="119"/>
+      <c r="W133" s="119"/>
+      <c r="X133" s="119"/>
+      <c r="Y133" s="119"/>
+      <c r="Z133" s="119"/>
+      <c r="AA133" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="AB133" s="93"/>
-      <c r="AC133" s="93"/>
+      <c r="AB133" s="120"/>
+      <c r="AC133" s="120"/>
     </row>
     <row r="134" spans="1:29">
       <c r="A134" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="B134" s="46">
-        <v>38246</v>
+      <c r="B134" s="124">
+        <v>37240</v>
       </c>
       <c r="C134" s="56"/>
       <c r="D134" s="71">
@@ -50608,8 +50659,8 @@
       <c r="A135" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B135" s="46">
-        <v>38307</v>
+      <c r="B135" s="124">
+        <v>37269</v>
       </c>
       <c r="C135" s="56"/>
       <c r="D135" s="71">
@@ -50648,8 +50699,8 @@
       <c r="A136" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="B136" s="46">
-        <v>38352</v>
+      <c r="B136" s="124">
+        <v>37304</v>
       </c>
       <c r="C136" s="56"/>
       <c r="D136" s="71">
@@ -50688,8 +50739,8 @@
       <c r="A137" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B137" s="46">
-        <v>38388</v>
+      <c r="B137" s="124">
+        <v>37328</v>
       </c>
       <c r="C137" s="56"/>
       <c r="D137" s="71">
@@ -50728,8 +50779,8 @@
       <c r="A138" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="B138" s="46">
-        <v>38417</v>
+      <c r="B138" s="124">
+        <v>37337</v>
       </c>
       <c r="C138" s="56"/>
       <c r="D138" s="71">
@@ -50768,8 +50819,8 @@
       <c r="A139" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B139" s="46">
-        <v>38531</v>
+      <c r="B139" s="124">
+        <v>37340</v>
       </c>
       <c r="C139" s="56"/>
       <c r="D139" s="71">
@@ -50808,8 +50859,8 @@
       <c r="A140" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B140" s="46">
-        <v>38538</v>
+      <c r="B140" s="124">
+        <v>37357</v>
       </c>
       <c r="C140" s="56"/>
       <c r="D140" s="71">
@@ -50848,8 +50899,8 @@
       <c r="A141" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="B141" s="46">
-        <v>38569</v>
+      <c r="B141" s="124">
+        <v>37378</v>
       </c>
       <c r="C141" s="56"/>
       <c r="D141" s="71">
@@ -50888,8 +50939,8 @@
       <c r="A142" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="B142" s="46">
-        <v>38605</v>
+      <c r="B142" s="124">
+        <v>37409</v>
       </c>
       <c r="C142" s="56"/>
       <c r="D142" s="71">
@@ -50928,8 +50979,8 @@
       <c r="A143" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="B143" s="46">
-        <v>38635</v>
+      <c r="B143" s="124">
+        <v>37439</v>
       </c>
       <c r="C143" s="56"/>
       <c r="D143" s="71">
@@ -50968,8 +51019,8 @@
       <c r="A144" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="B144" s="46">
-        <v>38660</v>
+      <c r="B144" s="124">
+        <v>37470</v>
       </c>
       <c r="C144" s="56"/>
       <c r="D144" s="71">
@@ -51008,8 +51059,8 @@
       <c r="A145" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="B145" s="46">
-        <v>38695</v>
+      <c r="B145" s="124">
+        <v>37500</v>
       </c>
       <c r="C145" s="56"/>
       <c r="D145" s="71">
@@ -51048,8 +51099,8 @@
       <c r="A146" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="B146" s="46">
-        <v>38726</v>
+      <c r="B146" s="124">
+        <v>37530</v>
       </c>
       <c r="C146" s="56"/>
       <c r="D146" s="71">
@@ -51088,8 +51139,8 @@
       <c r="A147" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B147" s="46">
-        <v>38755</v>
+      <c r="B147" s="124">
+        <v>37569</v>
       </c>
       <c r="C147" s="56"/>
       <c r="D147" s="71">
@@ -51128,8 +51179,8 @@
       <c r="A148" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B148" s="46">
-        <v>38782</v>
+      <c r="B148" s="124">
+        <v>37595</v>
       </c>
       <c r="C148" s="56"/>
       <c r="D148" s="71">
@@ -51168,8 +51219,8 @@
       <c r="A149" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="B149" s="46">
-        <v>38812</v>
+      <c r="B149" s="124">
+        <v>37629</v>
       </c>
       <c r="C149" s="56"/>
       <c r="D149" s="71">
@@ -51208,8 +51259,8 @@
       <c r="A150" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="B150" s="46">
-        <v>38842</v>
+      <c r="B150" s="124">
+        <v>37655</v>
       </c>
       <c r="C150" s="56"/>
       <c r="D150" s="71">
@@ -51248,8 +51299,8 @@
       <c r="A151" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="B151" s="46">
-        <v>38873</v>
+      <c r="B151" s="124">
+        <v>37686</v>
       </c>
       <c r="C151" s="56"/>
       <c r="D151" s="71">
@@ -51288,8 +51339,8 @@
       <c r="A152" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B152" s="46">
-        <v>38903</v>
+      <c r="B152" s="124">
+        <v>37716</v>
       </c>
       <c r="C152" s="56"/>
       <c r="D152" s="71">
@@ -51328,8 +51379,8 @@
       <c r="A153" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B153" s="46">
-        <v>38934</v>
+      <c r="B153" s="124">
+        <v>37750</v>
       </c>
       <c r="C153" s="56"/>
       <c r="D153" s="71">
@@ -51368,8 +51419,8 @@
       <c r="A154" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B154" s="46">
-        <v>38965</v>
+      <c r="B154" s="124">
+        <v>37784</v>
       </c>
       <c r="C154" s="56"/>
       <c r="D154" s="71">
@@ -51408,8 +51459,8 @@
       <c r="A155" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B155" s="46">
-        <v>38995</v>
+      <c r="B155" s="124">
+        <v>37818</v>
       </c>
       <c r="C155" s="56"/>
       <c r="D155" s="71">
@@ -51448,8 +51499,8 @@
       <c r="A156" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B156" s="46">
-        <v>39026</v>
+      <c r="B156" s="124">
+        <v>37853</v>
       </c>
       <c r="C156" s="56"/>
       <c r="D156" s="71">
@@ -51488,8 +51539,8 @@
       <c r="A157" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="B157" s="46">
-        <v>39056</v>
+      <c r="B157" s="124">
+        <v>37882</v>
       </c>
       <c r="C157" s="56"/>
       <c r="D157" s="71">
@@ -51528,8 +51579,8 @@
       <c r="A158" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="B158" s="46">
-        <v>39087</v>
+      <c r="B158" s="124">
+        <v>37924</v>
       </c>
       <c r="C158" s="56"/>
       <c r="D158" s="71">
@@ -51568,8 +51619,8 @@
       <c r="A159" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="B159" s="46">
-        <v>39118</v>
+      <c r="B159" s="124">
+        <v>37985</v>
       </c>
       <c r="C159" s="56"/>
       <c r="D159" s="71">
@@ -51608,8 +51659,8 @@
       <c r="A160" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="B160" s="46">
-        <v>39146</v>
+      <c r="B160" s="124">
+        <v>38048</v>
       </c>
       <c r="C160" s="56"/>
       <c r="D160" s="71">
@@ -51648,8 +51699,8 @@
       <c r="A161" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="B161" s="46">
-        <v>39177</v>
+      <c r="B161" s="124">
+        <v>38077</v>
       </c>
       <c r="C161" s="56"/>
       <c r="D161" s="71">
@@ -51688,8 +51739,8 @@
       <c r="A162" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="B162" s="46">
-        <v>39207</v>
+      <c r="B162" s="124">
+        <v>38107</v>
       </c>
       <c r="C162" s="56"/>
       <c r="D162" s="71">
@@ -51728,8 +51779,8 @@
       <c r="A163" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B163" s="46">
-        <v>39238</v>
+      <c r="B163" s="124">
+        <v>38140</v>
       </c>
       <c r="C163" s="56"/>
       <c r="D163" s="71">
@@ -51770,8 +51821,8 @@
       <c r="A164" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="B164" s="46">
-        <v>39268</v>
+      <c r="B164" s="124">
+        <v>38171</v>
       </c>
       <c r="C164" s="56"/>
       <c r="D164" s="71">
@@ -51812,8 +51863,8 @@
       <c r="A165" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="B165" s="46">
-        <v>39299</v>
+      <c r="B165" s="124">
+        <v>38215</v>
       </c>
       <c r="C165" s="56"/>
       <c r="D165" s="71">
@@ -51854,8 +51905,8 @@
       <c r="A166" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="B166" s="46">
-        <v>39330</v>
+      <c r="B166" s="124">
+        <v>38244</v>
       </c>
       <c r="C166" s="56"/>
       <c r="D166" s="71">
@@ -51896,8 +51947,8 @@
       <c r="A167" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="B167" s="46">
-        <v>39360</v>
+      <c r="B167" s="124">
+        <v>38303</v>
       </c>
       <c r="C167" s="56"/>
       <c r="D167" s="71">
@@ -51938,8 +51989,8 @@
       <c r="A168" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B168" s="46">
-        <v>39391</v>
+      <c r="B168" s="124">
+        <v>38351</v>
       </c>
       <c r="C168" s="56"/>
       <c r="D168" s="71">
@@ -51980,8 +52031,8 @@
       <c r="A169" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="B169" s="46">
-        <v>39421</v>
+      <c r="B169" s="124">
+        <v>38386</v>
       </c>
       <c r="C169" s="56"/>
       <c r="D169" s="71">
@@ -52022,8 +52073,8 @@
       <c r="A170" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="B170" s="46">
-        <v>39452</v>
+      <c r="B170" s="124">
+        <v>38416</v>
       </c>
       <c r="C170" s="56"/>
       <c r="D170" s="71">
@@ -52064,8 +52115,8 @@
       <c r="A171" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="B171" s="46">
-        <v>39483</v>
+      <c r="B171" s="124">
+        <v>38535</v>
       </c>
       <c r="C171" s="56"/>
       <c r="D171" s="70"/>
@@ -52104,8 +52155,8 @@
       <c r="A172" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="B172" s="46">
-        <v>39512</v>
+      <c r="B172" s="124">
+        <v>38539</v>
       </c>
       <c r="C172" s="56"/>
       <c r="D172" s="72">
@@ -52146,8 +52197,8 @@
       <c r="A173" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="B173" s="46">
-        <v>39543</v>
+      <c r="B173" s="124">
+        <v>38570</v>
       </c>
       <c r="C173" s="56"/>
       <c r="D173" s="72"/>
@@ -52186,8 +52237,8 @@
       <c r="A174" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="B174" s="46">
-        <v>39573</v>
+      <c r="B174" s="124">
+        <v>38605</v>
       </c>
       <c r="C174" s="56"/>
       <c r="D174" s="72">
@@ -52228,8 +52279,8 @@
       <c r="A175" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="B175" s="46">
-        <v>39665</v>
+      <c r="B175" s="124">
+        <v>38635</v>
       </c>
       <c r="C175" s="56"/>
       <c r="D175" s="72">
@@ -52270,8 +52321,8 @@
       <c r="A176" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="B176" s="46">
-        <v>39697</v>
+      <c r="B176" s="124">
+        <v>38661</v>
       </c>
       <c r="C176" s="56"/>
       <c r="D176" s="72">
@@ -52312,8 +52363,8 @@
       <c r="A177" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="B177" s="46">
-        <v>39729</v>
+      <c r="B177" s="124">
+        <v>38695</v>
       </c>
       <c r="C177" s="56"/>
       <c r="D177" s="72">
@@ -52354,7 +52405,9 @@
       <c r="A178" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="B178" s="46"/>
+      <c r="B178" s="124">
+        <v>38726</v>
+      </c>
       <c r="C178" s="56"/>
       <c r="D178" s="72">
         <v>85</v>
@@ -52387,7 +52440,9 @@
       <c r="A179" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B179" s="46"/>
+      <c r="B179" s="124">
+        <v>38754</v>
+      </c>
       <c r="C179" s="56"/>
       <c r="D179" s="72">
         <v>85</v>
@@ -52420,7 +52475,9 @@
       <c r="A180" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="B180" s="46"/>
+      <c r="B180" s="124">
+        <v>38783</v>
+      </c>
       <c r="C180" s="56"/>
       <c r="D180" s="72">
         <v>85</v>
@@ -52453,7 +52510,9 @@
       <c r="A181" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B181" s="46"/>
+      <c r="B181" s="124">
+        <v>38812</v>
+      </c>
       <c r="C181" s="56"/>
       <c r="D181" s="72">
         <v>87</v>
@@ -53213,25 +53272,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="Y108:Z108"/>
-    <mergeCell ref="U109:V109"/>
-    <mergeCell ref="W109:X109"/>
-    <mergeCell ref="Y109:Z109"/>
-    <mergeCell ref="U110:V110"/>
-    <mergeCell ref="W110:X110"/>
-    <mergeCell ref="Y110:Z110"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="U108:V108"/>
-    <mergeCell ref="W108:X108"/>
-    <mergeCell ref="AA128:AC128"/>
-    <mergeCell ref="R123:Z123"/>
-    <mergeCell ref="AA123:AC123"/>
-    <mergeCell ref="R115:Z122"/>
-    <mergeCell ref="AA115:AC122"/>
-    <mergeCell ref="R124:Z127"/>
-    <mergeCell ref="AA124:AC127"/>
+    <mergeCell ref="R129:Z131"/>
+    <mergeCell ref="AA129:AC131"/>
+    <mergeCell ref="R132:Z132"/>
+    <mergeCell ref="AA132:AC132"/>
+    <mergeCell ref="R133:Z133"/>
+    <mergeCell ref="AA133:AC133"/>
     <mergeCell ref="U111:V111"/>
     <mergeCell ref="W111:X111"/>
     <mergeCell ref="Y111:Z111"/>
@@ -53242,12 +53288,25 @@
     <mergeCell ref="U113:V113"/>
     <mergeCell ref="W113:X113"/>
     <mergeCell ref="Y113:Z113"/>
-    <mergeCell ref="R129:Z131"/>
-    <mergeCell ref="AA129:AC131"/>
-    <mergeCell ref="R132:Z132"/>
-    <mergeCell ref="AA132:AC132"/>
-    <mergeCell ref="R133:Z133"/>
-    <mergeCell ref="AA133:AC133"/>
+    <mergeCell ref="AA128:AC128"/>
+    <mergeCell ref="R123:Z123"/>
+    <mergeCell ref="AA123:AC123"/>
+    <mergeCell ref="R115:Z122"/>
+    <mergeCell ref="AA115:AC122"/>
+    <mergeCell ref="R124:Z127"/>
+    <mergeCell ref="AA124:AC127"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="U108:V108"/>
+    <mergeCell ref="W108:X108"/>
+    <mergeCell ref="Y108:Z108"/>
+    <mergeCell ref="U109:V109"/>
+    <mergeCell ref="W109:X109"/>
+    <mergeCell ref="Y109:Z109"/>
+    <mergeCell ref="U110:V110"/>
+    <mergeCell ref="W110:X110"/>
+    <mergeCell ref="Y110:Z110"/>
   </mergeCells>
   <pageMargins left="0.28000000000000003" right="0.27" top="0.16" bottom="0.19" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -53285,16 +53344,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="121"/>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="A1" s="122"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="2" spans="1:8" ht="18.75">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="121" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
@@ -53673,11 +53732,11 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="18.75">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="121" t="s">
         <v>144</v>
       </c>
-      <c r="B35" s="120"/>
-      <c r="C35" s="120"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="121"/>
     </row>
     <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="5" t="s">
@@ -53916,22 +53975,22 @@
       <c r="C57" s="4">
         <v>127.3</v>
       </c>
-      <c r="E57" s="121"/>
-      <c r="F57" s="121"/>
-      <c r="G57" s="121"/>
-      <c r="H57" s="121"/>
-      <c r="I57" s="121"/>
-      <c r="J57" s="121"/>
-      <c r="K57" s="121"/>
-      <c r="L57" s="121"/>
-      <c r="M57" s="121"/>
-      <c r="N57" s="121"/>
-      <c r="O57" s="121"/>
-      <c r="P57" s="121"/>
-      <c r="Q57" s="121"/>
-      <c r="R57" s="121"/>
-      <c r="S57" s="121"/>
-      <c r="T57" s="121"/>
+      <c r="E57" s="122"/>
+      <c r="F57" s="122"/>
+      <c r="G57" s="122"/>
+      <c r="H57" s="122"/>
+      <c r="I57" s="122"/>
+      <c r="J57" s="122"/>
+      <c r="K57" s="122"/>
+      <c r="L57" s="122"/>
+      <c r="M57" s="122"/>
+      <c r="N57" s="122"/>
+      <c r="O57" s="122"/>
+      <c r="P57" s="122"/>
+      <c r="Q57" s="122"/>
+      <c r="R57" s="122"/>
+      <c r="S57" s="122"/>
+      <c r="T57" s="122"/>
     </row>
     <row r="58" spans="1:20" ht="18.75">
       <c r="A58" s="6" t="s">
@@ -53943,24 +54002,24 @@
       <c r="C58" s="4">
         <v>127.2</v>
       </c>
-      <c r="E58" s="120" t="s">
+      <c r="E58" s="121" t="s">
         <v>167</v>
       </c>
-      <c r="F58" s="120"/>
-      <c r="G58" s="120"/>
-      <c r="H58" s="120"/>
-      <c r="I58" s="120"/>
-      <c r="J58" s="120"/>
-      <c r="K58" s="120"/>
-      <c r="L58" s="120"/>
-      <c r="M58" s="120"/>
-      <c r="N58" s="120"/>
-      <c r="O58" s="120"/>
-      <c r="P58" s="120"/>
-      <c r="Q58" s="120"/>
-      <c r="R58" s="120"/>
-      <c r="S58" s="120"/>
-      <c r="T58" s="120"/>
+      <c r="F58" s="121"/>
+      <c r="G58" s="121"/>
+      <c r="H58" s="121"/>
+      <c r="I58" s="121"/>
+      <c r="J58" s="121"/>
+      <c r="K58" s="121"/>
+      <c r="L58" s="121"/>
+      <c r="M58" s="121"/>
+      <c r="N58" s="121"/>
+      <c r="O58" s="121"/>
+      <c r="P58" s="121"/>
+      <c r="Q58" s="121"/>
+      <c r="R58" s="121"/>
+      <c r="S58" s="121"/>
+      <c r="T58" s="121"/>
     </row>
     <row r="59" spans="1:20" ht="15.75">
       <c r="A59" s="6" t="s">
@@ -54540,11 +54599,11 @@
       </c>
     </row>
     <row r="68" spans="1:20" ht="18.75">
-      <c r="A68" s="120" t="s">
+      <c r="A68" s="121" t="s">
         <v>198</v>
       </c>
-      <c r="B68" s="120"/>
-      <c r="C68" s="120"/>
+      <c r="B68" s="121"/>
+      <c r="C68" s="121"/>
       <c r="E68" s="29" t="s">
         <v>199</v>
       </c>
@@ -55075,11 +55134,11 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="18.75">
-      <c r="A101" s="120" t="s">
+      <c r="A101" s="121" t="s">
         <v>232</v>
       </c>
-      <c r="B101" s="120"/>
-      <c r="C101" s="120"/>
+      <c r="B101" s="121"/>
+      <c r="C101" s="121"/>
     </row>
     <row r="102" spans="1:3" ht="15.75">
       <c r="A102" s="5" t="s">
@@ -55430,11 +55489,11 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="18.75">
-      <c r="A134" s="120" t="s">
+      <c r="A134" s="121" t="s">
         <v>263</v>
       </c>
-      <c r="B134" s="120"/>
-      <c r="C134" s="120"/>
+      <c r="B134" s="121"/>
+      <c r="C134" s="121"/>
     </row>
     <row r="135" spans="1:3" ht="15.75">
       <c r="A135" s="5" t="s">
@@ -55781,11 +55840,11 @@
       </c>
     </row>
     <row r="167" spans="1:3" ht="18.75">
-      <c r="A167" s="120" t="s">
+      <c r="A167" s="121" t="s">
         <v>294</v>
       </c>
-      <c r="B167" s="120"/>
-      <c r="C167" s="120"/>
+      <c r="B167" s="121"/>
+      <c r="C167" s="121"/>
     </row>
     <row r="168" spans="1:3" ht="15.75">
       <c r="A168" s="5" t="s">
@@ -56136,11 +56195,11 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="18.75">
-      <c r="A200" s="120" t="s">
+      <c r="A200" s="121" t="s">
         <v>325</v>
       </c>
-      <c r="B200" s="120"/>
-      <c r="C200" s="120"/>
+      <c r="B200" s="121"/>
+      <c r="C200" s="121"/>
     </row>
     <row r="201" spans="1:3" ht="15.75">
       <c r="A201" s="5" t="s">
@@ -56472,11 +56531,11 @@
       </c>
     </row>
     <row r="232" spans="1:3" ht="18.75">
-      <c r="A232" s="120" t="s">
+      <c r="A232" s="121" t="s">
         <v>355</v>
       </c>
-      <c r="B232" s="120"/>
-      <c r="C232" s="120"/>
+      <c r="B232" s="121"/>
+      <c r="C232" s="121"/>
     </row>
     <row r="233" spans="1:3" ht="15.75">
       <c r="A233" s="5" t="s">
@@ -56820,11 +56879,11 @@
       </c>
     </row>
     <row r="264" spans="1:3" ht="18.75">
-      <c r="A264" s="120" t="s">
+      <c r="A264" s="121" t="s">
         <v>385</v>
       </c>
-      <c r="B264" s="120"/>
-      <c r="C264" s="120"/>
+      <c r="B264" s="121"/>
+      <c r="C264" s="121"/>
     </row>
     <row r="265" spans="1:3" ht="15.75">
       <c r="A265" s="5" t="s">
@@ -57164,11 +57223,11 @@
       </c>
     </row>
     <row r="296" spans="1:3" ht="18.75">
-      <c r="A296" s="120" t="s">
+      <c r="A296" s="121" t="s">
         <v>415</v>
       </c>
-      <c r="B296" s="120"/>
-      <c r="C296" s="120"/>
+      <c r="B296" s="121"/>
+      <c r="C296" s="121"/>
     </row>
     <row r="297" spans="1:3" ht="15.75">
       <c r="A297" s="5" t="s">
@@ -57512,11 +57571,11 @@
       </c>
     </row>
     <row r="328" spans="1:3" ht="18.75">
-      <c r="A328" s="120" t="s">
+      <c r="A328" s="121" t="s">
         <v>446</v>
       </c>
-      <c r="B328" s="120"/>
-      <c r="C328" s="120"/>
+      <c r="B328" s="121"/>
+      <c r="C328" s="121"/>
     </row>
     <row r="329" spans="1:3" ht="15.75">
       <c r="A329" s="5" t="s">
@@ -57860,11 +57919,11 @@
       </c>
     </row>
     <row r="360" spans="1:3" ht="18.75">
-      <c r="A360" s="120" t="s">
+      <c r="A360" s="121" t="s">
         <v>476</v>
       </c>
-      <c r="B360" s="120"/>
-      <c r="C360" s="120"/>
+      <c r="B360" s="121"/>
+      <c r="C360" s="121"/>
     </row>
     <row r="361" spans="1:3" ht="15.75">
       <c r="A361" s="5" t="s">
@@ -58190,6 +58249,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="E57:T57"/>
+    <mergeCell ref="E58:T58"/>
     <mergeCell ref="A296:C296"/>
     <mergeCell ref="A328:C328"/>
     <mergeCell ref="A360:C360"/>
@@ -58199,12 +58264,6 @@
     <mergeCell ref="A167:C167"/>
     <mergeCell ref="A200:C200"/>
     <mergeCell ref="A232:C232"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="E57:T57"/>
-    <mergeCell ref="E58:T58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -58244,16 +58303,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="121"/>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="A1" s="122"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="2" spans="1:8" ht="18.75">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="121" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
@@ -58632,11 +58691,11 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="18.75">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="121" t="s">
         <v>144</v>
       </c>
-      <c r="B35" s="120"/>
-      <c r="C35" s="120"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="121"/>
     </row>
     <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="29" t="s">
@@ -58879,22 +58938,22 @@
       <c r="C57" s="4">
         <v>119.7</v>
       </c>
-      <c r="E57" s="121"/>
-      <c r="F57" s="121"/>
-      <c r="G57" s="121"/>
-      <c r="H57" s="121"/>
-      <c r="I57" s="121"/>
-      <c r="J57" s="121"/>
-      <c r="K57" s="121"/>
-      <c r="L57" s="121"/>
-      <c r="M57" s="121"/>
-      <c r="N57" s="121"/>
-      <c r="O57" s="121"/>
-      <c r="P57" s="121"/>
-      <c r="Q57" s="121"/>
-      <c r="R57" s="121"/>
-      <c r="S57" s="121"/>
-      <c r="T57" s="121"/>
+      <c r="E57" s="122"/>
+      <c r="F57" s="122"/>
+      <c r="G57" s="122"/>
+      <c r="H57" s="122"/>
+      <c r="I57" s="122"/>
+      <c r="J57" s="122"/>
+      <c r="K57" s="122"/>
+      <c r="L57" s="122"/>
+      <c r="M57" s="122"/>
+      <c r="N57" s="122"/>
+      <c r="O57" s="122"/>
+      <c r="P57" s="122"/>
+      <c r="Q57" s="122"/>
+      <c r="R57" s="122"/>
+      <c r="S57" s="122"/>
+      <c r="T57" s="122"/>
     </row>
     <row r="58" spans="1:20" ht="18.75">
       <c r="A58" s="29" t="s">
@@ -58906,24 +58965,24 @@
       <c r="C58" s="4">
         <v>119.1</v>
       </c>
-      <c r="E58" s="120" t="s">
+      <c r="E58" s="121" t="s">
         <v>167</v>
       </c>
-      <c r="F58" s="120"/>
-      <c r="G58" s="120"/>
-      <c r="H58" s="120"/>
-      <c r="I58" s="120"/>
-      <c r="J58" s="120"/>
-      <c r="K58" s="120"/>
-      <c r="L58" s="120"/>
-      <c r="M58" s="120"/>
-      <c r="N58" s="120"/>
-      <c r="O58" s="120"/>
-      <c r="P58" s="120"/>
-      <c r="Q58" s="120"/>
-      <c r="R58" s="120"/>
-      <c r="S58" s="120"/>
-      <c r="T58" s="120"/>
+      <c r="F58" s="121"/>
+      <c r="G58" s="121"/>
+      <c r="H58" s="121"/>
+      <c r="I58" s="121"/>
+      <c r="J58" s="121"/>
+      <c r="K58" s="121"/>
+      <c r="L58" s="121"/>
+      <c r="M58" s="121"/>
+      <c r="N58" s="121"/>
+      <c r="O58" s="121"/>
+      <c r="P58" s="121"/>
+      <c r="Q58" s="121"/>
+      <c r="R58" s="121"/>
+      <c r="S58" s="121"/>
+      <c r="T58" s="121"/>
     </row>
     <row r="59" spans="1:20" ht="15.75">
       <c r="A59" s="29" t="s">
@@ -59380,11 +59439,11 @@
       <c r="T67" s="16"/>
     </row>
     <row r="68" spans="1:20" ht="18.75">
-      <c r="A68" s="120" t="s">
+      <c r="A68" s="121" t="s">
         <v>198</v>
       </c>
-      <c r="B68" s="120"/>
-      <c r="C68" s="120"/>
+      <c r="B68" s="121"/>
+      <c r="C68" s="121"/>
       <c r="E68" s="6"/>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
@@ -59803,11 +59862,11 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="18.75">
-      <c r="A101" s="120" t="s">
+      <c r="A101" s="121" t="s">
         <v>232</v>
       </c>
-      <c r="B101" s="120"/>
-      <c r="C101" s="120"/>
+      <c r="B101" s="121"/>
+      <c r="C101" s="121"/>
     </row>
     <row r="102" spans="1:3" ht="15.75">
       <c r="A102" s="29" t="s">
@@ -60162,11 +60221,11 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="18.75">
-      <c r="A134" s="120" t="s">
+      <c r="A134" s="121" t="s">
         <v>263</v>
       </c>
-      <c r="B134" s="120"/>
-      <c r="C134" s="120"/>
+      <c r="B134" s="121"/>
+      <c r="C134" s="121"/>
     </row>
     <row r="135" spans="1:3" ht="15.75">
       <c r="A135" s="29" t="s">
@@ -60513,11 +60572,11 @@
       <c r="C166" s="4"/>
     </row>
     <row r="167" spans="1:3" ht="18.75">
-      <c r="A167" s="120" t="s">
+      <c r="A167" s="121" t="s">
         <v>294</v>
       </c>
-      <c r="B167" s="120"/>
-      <c r="C167" s="120"/>
+      <c r="B167" s="121"/>
+      <c r="C167" s="121"/>
     </row>
     <row r="168" spans="1:3" ht="15.75">
       <c r="A168" s="29" t="s">
@@ -60862,11 +60921,11 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="18.75">
-      <c r="A200" s="120" t="s">
+      <c r="A200" s="121" t="s">
         <v>325</v>
       </c>
-      <c r="B200" s="120"/>
-      <c r="C200" s="120"/>
+      <c r="B200" s="121"/>
+      <c r="C200" s="121"/>
     </row>
     <row r="201" spans="1:3" ht="15.75">
       <c r="A201" s="29" t="s">
@@ -61106,11 +61165,11 @@
       <c r="C231" s="4"/>
     </row>
     <row r="232" spans="1:3" ht="18.75">
-      <c r="A232" s="120" t="s">
+      <c r="A232" s="121" t="s">
         <v>355</v>
       </c>
-      <c r="B232" s="120"/>
-      <c r="C232" s="120"/>
+      <c r="B232" s="121"/>
+      <c r="C232" s="121"/>
     </row>
     <row r="233" spans="1:3" ht="15.75">
       <c r="A233" s="29" t="s">
@@ -61334,11 +61393,11 @@
       <c r="C263" s="4"/>
     </row>
     <row r="264" spans="1:3" ht="18.75">
-      <c r="A264" s="120" t="s">
+      <c r="A264" s="121" t="s">
         <v>385</v>
       </c>
-      <c r="B264" s="120"/>
-      <c r="C264" s="120"/>
+      <c r="B264" s="121"/>
+      <c r="C264" s="121"/>
     </row>
     <row r="265" spans="1:3" ht="15.75">
       <c r="A265" s="29" t="s">
@@ -61562,11 +61621,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="18.75">
-      <c r="A296" s="120" t="s">
+      <c r="A296" s="121" t="s">
         <v>415</v>
       </c>
-      <c r="B296" s="120"/>
-      <c r="C296" s="120"/>
+      <c r="B296" s="121"/>
+      <c r="C296" s="121"/>
     </row>
     <row r="297" spans="1:3" ht="15.75">
       <c r="A297" s="29" t="s">
@@ -61790,11 +61849,11 @@
       <c r="C327" s="4"/>
     </row>
     <row r="328" spans="1:3" ht="18.75">
-      <c r="A328" s="120" t="s">
+      <c r="A328" s="121" t="s">
         <v>446</v>
       </c>
-      <c r="B328" s="120"/>
-      <c r="C328" s="120"/>
+      <c r="B328" s="121"/>
+      <c r="C328" s="121"/>
     </row>
     <row r="329" spans="1:3" ht="15.75">
       <c r="A329" s="29" t="s">
@@ -62018,11 +62077,11 @@
       <c r="C359" s="4"/>
     </row>
     <row r="360" spans="1:3" ht="18.75">
-      <c r="A360" s="120" t="s">
+      <c r="A360" s="121" t="s">
         <v>476</v>
       </c>
-      <c r="B360" s="120"/>
-      <c r="C360" s="120"/>
+      <c r="B360" s="121"/>
+      <c r="C360" s="121"/>
     </row>
     <row r="361" spans="1:3" ht="15.75">
       <c r="A361" s="29" t="s">
@@ -62240,6 +62299,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E58:T58"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="E57:T57"/>
     <mergeCell ref="A264:C264"/>
     <mergeCell ref="A296:C296"/>
     <mergeCell ref="A328:C328"/>
@@ -62250,11 +62314,6 @@
     <mergeCell ref="A167:C167"/>
     <mergeCell ref="A200:C200"/>
     <mergeCell ref="A232:C232"/>
-    <mergeCell ref="E58:T58"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="E57:T57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>